<commit_message>
completed record day 2
</commit_message>
<xml_diff>
--- a/Parametrize/Default.xlsx
+++ b/Parametrize/Default.xlsx
@@ -469,7 +469,9 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>

</xml_diff>